<commit_message>
Dopsani dalšího textu k dotazníku
</commit_message>
<xml_diff>
--- a/Dotaznik/Dotazník užívání webové aplikace Diani (Odpovědi).xlsx
+++ b/Dotaznik/Dotazník užívání webové aplikace Diani (Odpovědi).xlsx
@@ -568,9 +568,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S11" sqref="S11"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Přidány úpravy podle Albertova
</commit_message>
<xml_diff>
--- a/Dotaznik/Dotazník užívání webové aplikace Diani (Odpovědi).xlsx
+++ b/Dotaznik/Dotazník užívání webové aplikace Diani (Odpovědi).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9615" windowHeight="5250"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9615" windowHeight="5250" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Odpovědi formuláře 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
   <si>
     <t>Pohlaví</t>
   </si>
@@ -239,6 +239,15 @@
   </si>
   <si>
     <t>chytrý telefon (Smartphone)</t>
+  </si>
+  <si>
+    <t>prum</t>
+  </si>
+  <si>
+    <t>vyb prum</t>
+  </si>
+  <si>
+    <t>var</t>
   </si>
 </sst>
 </file>
@@ -568,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
@@ -999,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8:M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1266,6 +1275,9 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
       <c r="H7">
         <f>AVERAGE(H2:H6)</f>
         <v>4.4000000000000004</v>
@@ -1291,33 +1303,66 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="H9">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8">
+        <f>_xlfn.VAR.S(H2:H6)</f>
+        <v>0.80000000000000071</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ref="I8:M8" si="1">_xlfn.VAR.S(I2:I6)</f>
+        <v>3.3000000000000007</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="1"/>
+        <v>1.2999999999999998</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>0.19999999999999929</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>0.70000000000000018</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>73</v>
+      </c>
+      <c r="H10">
         <f>AVERAGE(H3:H5)</f>
         <v>4</v>
       </c>
-      <c r="I9">
-        <f t="shared" ref="I9:M9" si="1">AVERAGE(I3:I5)</f>
-        <v>4</v>
-      </c>
-      <c r="J9">
-        <f t="shared" si="1"/>
+      <c r="I10">
+        <f>AVERAGE(I3:I5)</f>
+        <v>4</v>
+      </c>
+      <c r="J10">
+        <f>AVERAGE(J3:J5)</f>
         <v>2.3333333333333335</v>
       </c>
-      <c r="K9">
-        <f t="shared" si="1"/>
+      <c r="K10">
+        <f>AVERAGE(K3:K5)</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="L9">
-        <f t="shared" si="1"/>
+      <c r="L10">
+        <f>AVERAGE(L3:L5)</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="M9">
-        <f t="shared" si="1"/>
+      <c r="M10">
+        <f>AVERAGE(M3:M5)</f>
         <v>1.6666666666666667</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Upraveny obrázky Doplněny dotazníky 2/3 (chybí obrázky)
</commit_message>
<xml_diff>
--- a/Dotaznik/Dotazník užívání webové aplikace Diani (Odpovědi).xlsx
+++ b/Dotaznik/Dotazník užívání webové aplikace Diani (Odpovědi).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milhouse\Documents\Scholla\___FEL\22rocnik\Diplomova práce\Dotaznik\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milhouse\Documents\Scholla\___FEL\Diplomova práce\Dotaznik\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="9615" windowHeight="5250" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11745"/>
   </bookViews>
   <sheets>
     <sheet name="Odpovědi formuláře 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="104">
   <si>
     <t>Pohlaví</t>
   </si>
@@ -248,13 +248,103 @@
   </si>
   <si>
     <t>var</t>
+  </si>
+  <si>
+    <t>med</t>
+  </si>
+  <si>
+    <t>Nejsem diabetik</t>
+  </si>
+  <si>
+    <t>cca 1 rok</t>
+  </si>
+  <si>
+    <t>1 rok</t>
+  </si>
+  <si>
+    <t>1 týden</t>
+  </si>
+  <si>
+    <t>Aplikace inzulínu pomocí inzulínové pumpy</t>
+  </si>
+  <si>
+    <t>Aplikace inzulínu perem</t>
+  </si>
+  <si>
+    <t>nejsem diabetik</t>
+  </si>
+  <si>
+    <t>modus</t>
+  </si>
+  <si>
+    <t>ca rok</t>
+  </si>
+  <si>
+    <t>2x týdně</t>
+  </si>
+  <si>
+    <t>Ke sledování souvislostí mezi naměřenými daty</t>
+  </si>
+  <si>
+    <t>obe vyse uvedene, spise diani</t>
+  </si>
+  <si>
+    <t>stačí mi informace z aplikace Diabetesdagboka zobrazované na chytrém telefonu (Smartphone).</t>
+  </si>
+  <si>
+    <t>Možnost propojit a zobrazit data z více zařízení</t>
+  </si>
+  <si>
+    <t>Nevim</t>
+  </si>
+  <si>
+    <t>Uživatelské (odesílání pošty, prohlížení web. stránek...)</t>
+  </si>
+  <si>
+    <t>Rok</t>
+  </si>
+  <si>
+    <t>Denne</t>
+  </si>
+  <si>
+    <t>K tisku diabetického deníku</t>
+  </si>
+  <si>
+    <t>Chytrý telefon (Smartphone) pomocí aplikace Diabetesdagboka</t>
+  </si>
+  <si>
+    <t>Přehledné tabulky</t>
+  </si>
+  <si>
+    <t>Infografiku (grafy, tabulky)</t>
+  </si>
+  <si>
+    <t>nevím</t>
+  </si>
+  <si>
+    <t>týden</t>
+  </si>
+  <si>
+    <t>1x týdně</t>
+  </si>
+  <si>
+    <t>nemám potřebu analyzovat data., nejsem diabetik</t>
+  </si>
+  <si>
+    <t>Zpracování grafů, Přehledné tabulky, Exporty dat</t>
+  </si>
+  <si>
+    <t>Nic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -263,6 +353,19 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -285,15 +388,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -575,449 +692,658 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <selection pane="bottomLeft" activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="23" width="21.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="6.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="23" width="21.5703125" style="9" customWidth="1"/>
+    <col min="24" max="16384" width="14.42578125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="E1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="G1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="5">
         <v>55</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="1">
-        <v>5</v>
-      </c>
-      <c r="N2" s="1">
+      <c r="M2" s="5">
+        <v>5</v>
+      </c>
+      <c r="N2" s="5">
         <v>1</v>
       </c>
-      <c r="O2" s="1">
+      <c r="O2" s="5">
         <v>1</v>
       </c>
-      <c r="P2" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>3</v>
-      </c>
-      <c r="R2" s="1">
-        <v>3</v>
-      </c>
-      <c r="S2" s="1" t="s">
+      <c r="P2" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>3</v>
+      </c>
+      <c r="R2" s="5">
+        <v>3</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="5">
         <v>41</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="5">
         <v>4</v>
       </c>
-      <c r="N3" s="1">
-        <v>5</v>
-      </c>
-      <c r="O3" s="1">
-        <v>3</v>
-      </c>
-      <c r="P3" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>3</v>
-      </c>
-      <c r="R3" s="1">
+      <c r="N3" s="5">
+        <v>5</v>
+      </c>
+      <c r="O3" s="5">
+        <v>3</v>
+      </c>
+      <c r="P3" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>3</v>
+      </c>
+      <c r="R3" s="5">
         <v>2</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="T3" s="1" t="s">
+      <c r="T3" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U3" s="1" t="s">
+      <c r="U3" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V3" s="1" t="s">
+      <c r="V3" s="5" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="5">
         <v>65</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="M4" s="1">
-        <v>5</v>
-      </c>
-      <c r="N4" s="1">
-        <v>5</v>
-      </c>
-      <c r="O4" s="1">
+      <c r="M4" s="5">
+        <v>5</v>
+      </c>
+      <c r="N4" s="5">
+        <v>5</v>
+      </c>
+      <c r="O4" s="5">
         <v>2</v>
       </c>
-      <c r="P4" s="1">
+      <c r="P4" s="5">
         <v>2</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="Q4" s="5">
         <v>4</v>
       </c>
-      <c r="R4" s="1">
+      <c r="R4" s="5">
         <v>2</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" s="5" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="5">
         <v>58</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="M5" s="1">
-        <v>3</v>
-      </c>
-      <c r="N5" s="1">
+      <c r="M5" s="5">
+        <v>3</v>
+      </c>
+      <c r="N5" s="5">
         <v>2</v>
       </c>
-      <c r="O5" s="1">
+      <c r="O5" s="5">
         <v>2</v>
       </c>
-      <c r="P5" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>3</v>
-      </c>
-      <c r="R5" s="1">
+      <c r="P5" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q5" s="5">
+        <v>3</v>
+      </c>
+      <c r="R5" s="5">
         <v>1</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="5" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="5">
         <v>65</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="1">
-        <v>5</v>
-      </c>
-      <c r="N6" s="1">
+      <c r="M6" s="5">
+        <v>5</v>
+      </c>
+      <c r="N6" s="5">
         <v>4</v>
       </c>
-      <c r="O6" s="1">
+      <c r="O6" s="5">
         <v>4</v>
       </c>
-      <c r="P6" s="1">
+      <c r="P6" s="5">
         <v>4</v>
       </c>
-      <c r="Q6" s="1">
-        <v>3</v>
-      </c>
-      <c r="R6" s="1">
-        <v>3</v>
-      </c>
-      <c r="S6" s="1" t="s">
+      <c r="Q6" s="5">
+        <v>3</v>
+      </c>
+      <c r="R6" s="5">
+        <v>3</v>
+      </c>
+      <c r="S6" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="5" t="s">
         <v>64</v>
       </c>
+    </row>
+    <row r="7" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="12">
+        <v>50</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="M7" s="12">
+        <v>5</v>
+      </c>
+      <c r="N7" s="12">
+        <v>1</v>
+      </c>
+      <c r="O7" s="12">
+        <v>5</v>
+      </c>
+      <c r="P7" s="12">
+        <v>5</v>
+      </c>
+      <c r="Q7" s="12">
+        <v>3</v>
+      </c>
+      <c r="R7" s="12">
+        <v>1</v>
+      </c>
+      <c r="S7" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="T7" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="U7" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="V7" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="W7" s="11"/>
+    </row>
+    <row r="8" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="M8" s="12">
+        <v>5</v>
+      </c>
+      <c r="N8" s="12">
+        <v>1</v>
+      </c>
+      <c r="O8" s="12">
+        <v>5</v>
+      </c>
+      <c r="P8" s="12">
+        <v>5</v>
+      </c>
+      <c r="Q8" s="12">
+        <v>5</v>
+      </c>
+      <c r="R8" s="12">
+        <v>1</v>
+      </c>
+      <c r="S8" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="T8" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="U8" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="V8" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="W8" s="11"/>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="M9" s="12">
+        <v>3</v>
+      </c>
+      <c r="N9" s="12">
+        <v>5</v>
+      </c>
+      <c r="O9" s="12">
+        <v>3</v>
+      </c>
+      <c r="P9" s="12">
+        <v>3</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>5</v>
+      </c>
+      <c r="R9" s="12">
+        <v>3</v>
+      </c>
+      <c r="S9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="T9" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="U9" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="V9" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="W9" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8:M8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" customWidth="1"/>
@@ -1028,7 +1354,7 @@
     <col min="12" max="12" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>66</v>
       </c>
@@ -1070,294 +1396,520 @@
       </c>
     </row>
     <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="4">
         <v>1</v>
       </c>
-      <c r="H2" s="1">
-        <v>5</v>
-      </c>
-      <c r="I2" s="1">
+      <c r="H2" s="5">
+        <v>5</v>
+      </c>
+      <c r="I2" s="5">
         <v>1</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="5">
         <v>1</v>
       </c>
-      <c r="K2" s="1">
-        <v>3</v>
-      </c>
-      <c r="L2" s="1">
-        <v>3</v>
-      </c>
-      <c r="M2" s="1">
+      <c r="K2" s="5">
+        <v>3</v>
+      </c>
+      <c r="L2" s="5">
+        <v>3</v>
+      </c>
+      <c r="M2" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="4">
         <v>2</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="5">
         <v>4</v>
       </c>
-      <c r="I3" s="1">
-        <v>5</v>
-      </c>
-      <c r="J3" s="1">
-        <v>3</v>
-      </c>
-      <c r="K3" s="1">
-        <v>3</v>
-      </c>
-      <c r="L3" s="1">
-        <v>3</v>
-      </c>
-      <c r="M3" s="1">
+      <c r="I3" s="5">
+        <v>5</v>
+      </c>
+      <c r="J3" s="5">
+        <v>3</v>
+      </c>
+      <c r="K3" s="5">
+        <v>3</v>
+      </c>
+      <c r="L3" s="5">
+        <v>3</v>
+      </c>
+      <c r="M3" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="G4" s="2">
-        <v>3</v>
-      </c>
-      <c r="H4" s="1">
-        <v>5</v>
-      </c>
-      <c r="I4" s="1">
-        <v>5</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="G4" s="4">
+        <v>3</v>
+      </c>
+      <c r="H4" s="5">
+        <v>5</v>
+      </c>
+      <c r="I4" s="5">
+        <v>5</v>
+      </c>
+      <c r="J4" s="5">
         <v>2</v>
       </c>
-      <c r="K4" s="1">
+      <c r="K4" s="5">
         <v>2</v>
       </c>
-      <c r="L4" s="1">
+      <c r="L4" s="5">
         <v>4</v>
       </c>
-      <c r="M4" s="1">
+      <c r="M4" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="4">
         <v>4</v>
       </c>
-      <c r="H5" s="1">
-        <v>3</v>
-      </c>
-      <c r="I5" s="1">
+      <c r="H5" s="5">
+        <v>3</v>
+      </c>
+      <c r="I5" s="5">
         <v>2</v>
       </c>
-      <c r="J5" s="1">
+      <c r="J5" s="5">
         <v>2</v>
       </c>
-      <c r="K5" s="1">
-        <v>3</v>
-      </c>
-      <c r="L5" s="1">
-        <v>3</v>
-      </c>
-      <c r="M5" s="1">
+      <c r="K5" s="5">
+        <v>3</v>
+      </c>
+      <c r="L5" s="5">
+        <v>3</v>
+      </c>
+      <c r="M5" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="G6" s="2">
-        <v>5</v>
-      </c>
-      <c r="H6" s="1">
-        <v>5</v>
-      </c>
-      <c r="I6" s="1">
+      <c r="G6" s="4">
+        <v>5</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5</v>
+      </c>
+      <c r="I6" s="5">
         <v>4</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="5">
         <v>4</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="5">
         <v>4</v>
       </c>
-      <c r="L6" s="1">
-        <v>3</v>
-      </c>
-      <c r="M6" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G7" t="s">
+      <c r="L6" s="5">
+        <v>3</v>
+      </c>
+      <c r="M6" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="8">
+        <v>6</v>
+      </c>
+      <c r="H7" s="7">
+        <v>5</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>5</v>
+      </c>
+      <c r="K7" s="7">
+        <v>5</v>
+      </c>
+      <c r="L7" s="7">
+        <v>3</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G8" s="2">
+        <v>7</v>
+      </c>
+      <c r="H8" s="7">
+        <v>5</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <v>5</v>
+      </c>
+      <c r="K8" s="7">
+        <v>5</v>
+      </c>
+      <c r="L8" s="7">
+        <v>5</v>
+      </c>
+      <c r="M8" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="2">
+        <v>8</v>
+      </c>
+      <c r="H9" s="7">
+        <v>3</v>
+      </c>
+      <c r="I9" s="7">
+        <v>5</v>
+      </c>
+      <c r="J9" s="7">
+        <v>3</v>
+      </c>
+      <c r="K9" s="7">
+        <v>3</v>
+      </c>
+      <c r="L9" s="7">
+        <v>5</v>
+      </c>
+      <c r="M9" s="7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="H7">
-        <f>AVERAGE(H2:H6)</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="I7">
-        <f t="shared" ref="I7:M7" si="0">AVERAGE(I2:I6)</f>
-        <v>3.4</v>
-      </c>
-      <c r="J7">
+      <c r="H10" s="10">
+        <f>AVERAGE(H2:H9)</f>
+        <v>4.375</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" ref="I10:M10" si="0">AVERAGE(I2:I9)</f>
+        <v>3</v>
+      </c>
+      <c r="J10" s="10">
         <f t="shared" si="0"/>
-        <v>2.4</v>
-      </c>
-      <c r="K7">
+        <v>3.125</v>
+      </c>
+      <c r="K10" s="10">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="L7">
+        <v>3.5</v>
+      </c>
+      <c r="L10" s="10">
         <f t="shared" si="0"/>
-        <v>3.2</v>
-      </c>
-      <c r="M7">
+        <v>3.625</v>
+      </c>
+      <c r="M10" s="10">
         <f t="shared" si="0"/>
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="H8">
-        <f>_xlfn.VAR.S(H2:H6)</f>
-        <v>0.80000000000000071</v>
-      </c>
-      <c r="I8">
-        <f t="shared" ref="I8:M8" si="1">_xlfn.VAR.S(I2:I6)</f>
-        <v>3.3000000000000007</v>
-      </c>
-      <c r="J8">
+      <c r="H11" s="10">
+        <f>_xlfn.VAR.S(H2:H9)</f>
+        <v>0.8392857142857143</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" ref="I11:M11" si="1">_xlfn.VAR.S(I2:I9)</f>
+        <v>3.7142857142857144</v>
+      </c>
+      <c r="J11" s="10">
         <f t="shared" si="1"/>
-        <v>1.2999999999999998</v>
-      </c>
-      <c r="K8">
+        <v>2.125</v>
+      </c>
+      <c r="K11" s="10">
         <f t="shared" si="1"/>
-        <v>0.5</v>
-      </c>
-      <c r="L8">
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="L11" s="10">
         <f t="shared" si="1"/>
-        <v>0.19999999999999929</v>
-      </c>
-      <c r="M8">
+        <v>0.8392857142857143</v>
+      </c>
+      <c r="M11" s="10">
         <f t="shared" si="1"/>
-        <v>0.70000000000000018</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G10" t="s">
+        <v>0.8571428571428571</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="H12" s="10">
+        <f>MODE(H2:H9)</f>
+        <v>5</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" ref="I12:M12" si="2">MODE(I2:I9)</f>
+        <v>1</v>
+      </c>
+      <c r="J12" s="10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="K12" s="10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="L12" s="10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M12" s="10">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="9">
+        <f>MEDIAN(H2:H9)</f>
+        <v>5</v>
+      </c>
+      <c r="I13" s="9">
+        <f t="shared" ref="I13:M13" si="3">MEDIAN(I2:I9)</f>
+        <v>3</v>
+      </c>
+      <c r="J13" s="9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="K13" s="9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="L13" s="9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="M13" s="9">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="H10">
-        <f>AVERAGE(H3:H5)</f>
+      <c r="H15" s="9">
+        <f t="shared" ref="H15:M15" si="4">AVERAGE(H3:H5)</f>
         <v>4</v>
       </c>
-      <c r="I10">
-        <f>AVERAGE(I3:I5)</f>
+      <c r="I15" s="9">
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="J10">
-        <f>AVERAGE(J3:J5)</f>
+      <c r="J15" s="9">
+        <f t="shared" si="4"/>
         <v>2.3333333333333335</v>
       </c>
-      <c r="K10">
-        <f>AVERAGE(K3:K5)</f>
+      <c r="K15" s="9">
+        <f t="shared" si="4"/>
         <v>2.6666666666666665</v>
       </c>
-      <c r="L10">
-        <f>AVERAGE(L3:L5)</f>
+      <c r="L15" s="9">
+        <f t="shared" si="4"/>
         <v>3.3333333333333335</v>
       </c>
-      <c r="M10">
-        <f>AVERAGE(M3:M5)</f>
+      <c r="M15" s="9">
+        <f t="shared" si="4"/>
         <v>1.6666666666666667</v>
       </c>
     </row>

</xml_diff>